<commit_message>
Data provider for Car search added
</commit_message>
<xml_diff>
--- a/src/test/resources/TestDataForCarSearch.xlsx
+++ b/src/test/resources/TestDataForCarSearch.xlsx
@@ -1,21 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\walia\eclipse-workspace\PracticeProject\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{33505A9D-6829-4F18-8475-D2B0BFF0D4B7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53B51F47-61B5-415C-BDBE-F0DB9C2A9A74}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{88DD8342-192F-4C92-89AE-276DA9670437}"/>
+    <workbookView xWindow="384" yWindow="384" windowWidth="17280" windowHeight="8964" xr2:uid="{88DD8342-192F-4C92-89AE-276DA9670437}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -33,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="14">
   <si>
     <t>PickUpLocation</t>
   </si>
@@ -60,6 +61,21 @@
   </si>
   <si>
     <t>4.00 pm</t>
+  </si>
+  <si>
+    <t>07/20/2020</t>
+  </si>
+  <si>
+    <t>07/25/2020</t>
+  </si>
+  <si>
+    <t>07/22/2020</t>
+  </si>
+  <si>
+    <t>08/30/2020</t>
+  </si>
+  <si>
+    <t>07/30/2020</t>
   </si>
 </sst>
 </file>
@@ -95,9 +111,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -415,83 +436,84 @@
   <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="15.88671875" customWidth="1"/>
-    <col min="2" max="2" width="13" customWidth="1"/>
-    <col min="3" max="3" width="12.44140625" customWidth="1"/>
+    <col min="2" max="2" width="15.109375" customWidth="1"/>
+    <col min="3" max="3" width="16.33203125" customWidth="1"/>
     <col min="4" max="4" width="15.21875" customWidth="1"/>
     <col min="5" max="5" width="12.21875" customWidth="1"/>
+    <col min="6" max="6" width="12.109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
+      <c r="A2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="1">
-        <v>44014</v>
-      </c>
-      <c r="C2" t="s">
+      <c r="B2" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="1">
-        <v>44022</v>
-      </c>
-      <c r="E2" t="s">
+      <c r="D2" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E2" s="1" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
+      <c r="A3" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="1">
-        <v>44014</v>
-      </c>
-      <c r="C3" t="s">
+      <c r="B3" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="D3" s="1">
-        <v>44024</v>
-      </c>
-      <c r="E3" t="s">
+      <c r="D3" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E3" s="1" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
+      <c r="A4" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="1">
-        <v>44014</v>
-      </c>
-      <c r="C4" t="s">
+      <c r="B4" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D4" s="1">
-        <v>44025</v>
-      </c>
-      <c r="E4" t="s">
+      <c r="D4" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E4" s="1" t="s">
         <v>6</v>
       </c>
     </row>

</xml_diff>